<commit_message>
Removed Reporter log changed testing.Xml
</commit_message>
<xml_diff>
--- a/DataDrivenProject/src/test/resources/excel/project1.xlsx
+++ b/DataDrivenProject/src/test/resources/excel/project1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathiyananddharmaraj/Desktop/eclipse-workspace/DataDrivenProject/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathiyananddharmaraj/git/DataDrivenProject1/DataDrivenProject/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADDE770-6A64-8A4F-9DA8-3A4ECA854FC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABBB42C-5A1C-D143-A0E4-E2560DDD4AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{AC2FBF9F-7AB7-564B-9370-703811A09D42}"/>
   </bookViews>
@@ -104,13 +104,13 @@
     <t>firstName</t>
   </si>
   <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Mike123</t>
-  </si>
-  <si>
-    <t>Customer</t>
+    <t>Customer Created</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Bill123</t>
   </si>
 </sst>
 </file>
@@ -489,12 +489,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -537,7 +538,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -561,7 +562,7 @@
         <v>328967</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>12</v>
@@ -570,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>